<commit_message>
Stats adicionado ao orchestration
</commit_message>
<xml_diff>
--- a/Back-End/Schemas.xlsx
+++ b/Back-End/Schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/Desktop/fcul/AW/aw-project/Back-End/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Desktop\Faculdade\AW\aw-project\Back-End\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD579DF-35F8-7449-B546-BFCAED118873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CA8843-D6A1-44DC-AC78-56526A1AFB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{44408B4A-D2D9-4F42-9D55-C708D3E7EF91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44408B4A-D2D9-4F42-9D55-C708D3E7EF91}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Market: {id, name, location}</t>
   </si>
   <si>
-    <t>Stats: {id, [stats]}</t>
-  </si>
-  <si>
     <t>News: {id, title, author, text}</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>Feedback: {id, product_id, user_id, score}</t>
+  </si>
+  <si>
+    <t>Stats: {id, [statistics]}</t>
   </si>
 </sst>
 </file>
@@ -249,9 +249,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -259,6 +256,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -598,20 +598,20 @@
   <dimension ref="D5:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="55.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:12" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,18 +624,18 @@
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D6" s="2" t="s">
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="1"/>
@@ -643,12 +643,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D7" s="2"/>
-      <c r="E7" s="4" t="s">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+      <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="1"/>
@@ -656,122 +656,122 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D8" s="2"/>
-      <c r="E8" s="4" t="s">
+    <row r="8" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+      <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D9" s="2"/>
-      <c r="E9" s="4" t="s">
+    <row r="9" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="L9" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D10" s="2" t="s">
+      <c r="L9" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D11" s="2"/>
-      <c r="E11" s="4" t="s">
+      <c r="L10" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D12" s="2"/>
-      <c r="E12" s="4" t="s">
+      <c r="L11" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D13" s="2"/>
-      <c r="E13" s="4" t="s">
+    <row r="13" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="E13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="L13" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="D14" s="2"/>
-      <c r="E14" s="4" t="s">
+      <c r="L13" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+      <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="L14" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D15" s="2"/>
-      <c r="E15" s="4" t="s">
+      <c r="L14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="6"/>
+      <c r="E15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -779,14 +779,14 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D16" s="2" t="s">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="1"/>
@@ -794,12 +794,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D17" s="2"/>
-      <c r="E17" s="4" t="s">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="6"/>
+      <c r="E17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="1"/>
@@ -807,23 +807,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D18" s="2"/>
-      <c r="E18" s="4" t="s">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="6"/>
+      <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-      <c r="E19" s="4" t="s">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="6"/>
+      <c r="E19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -831,12 +831,12 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="2"/>
-      <c r="E20" s="4" t="s">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="6"/>
+      <c r="E20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -844,14 +844,14 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D21" s="2" t="s">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="1"/>
@@ -859,12 +859,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D22" s="2"/>
-      <c r="E22" s="4" t="s">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="6"/>
+      <c r="E22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -872,12 +872,12 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D23" s="2"/>
-      <c r="E23" s="4" t="s">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="6"/>
+      <c r="E23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -885,14 +885,14 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -900,14 +900,14 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D25" s="2" t="s">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -915,12 +915,12 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D26" s="2"/>
-      <c r="E26" s="4" t="s">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="6"/>
+      <c r="E26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -928,12 +928,12 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D27" s="2"/>
-      <c r="E27" s="4" t="s">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="6"/>
+      <c r="E27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -941,12 +941,12 @@
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D28" s="2"/>
-      <c r="E28" s="4" t="s">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="6"/>
+      <c r="E28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -954,14 +954,14 @@
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D29" s="2" t="s">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G29" s="1"/>
@@ -969,12 +969,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D30" s="2"/>
-      <c r="E30" s="4" t="s">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="6"/>
+      <c r="E30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="1"/>
@@ -982,23 +982,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D31" s="2"/>
-      <c r="E31" s="4" t="s">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="6"/>
+      <c r="E31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D32" s="2"/>
-      <c r="E32" s="4" t="s">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="6"/>
+      <c r="E32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -1008,12 +1008,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D29:D32"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="D10:D15"/>
     <mergeCell ref="D16:D20"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="D25:D28"/>
-    <mergeCell ref="D29:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>